<commit_message>
Robot program w/out plc is, i suppose, ready
</commit_message>
<xml_diff>
--- a/Таблица сигналов.xlsx
+++ b/Таблица сигналов.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SW002-LoadWizardPro_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CAB4F0-E4B2-447A-8D6B-92D761468989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA87A445-B61D-4490-8F27-FF840CA6F0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="4368" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{0F8F6BBE-EBD7-4FEB-A239-792B86B6C8F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0F8F6BBE-EBD7-4FEB-A239-792B86B6C8F6}"/>
   </bookViews>
   <sheets>
     <sheet name="IO ПЛК" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="372">
   <si>
     <t>Комментарий</t>
   </si>
@@ -868,18 +868,6 @@
     <t>Скорость робота</t>
   </si>
   <si>
-    <t>Полка 1 в работе</t>
-  </si>
-  <si>
-    <t>Полка 2 в работе</t>
-  </si>
-  <si>
-    <t>Полка 3 в работе</t>
-  </si>
-  <si>
-    <t>Полка 4 в работе</t>
-  </si>
-  <si>
     <t>Захват 1 датчик сработал</t>
   </si>
   <si>
@@ -1106,6 +1094,66 @@
   </si>
   <si>
     <t>ID пластины в базе данных</t>
+  </si>
+  <si>
+    <t>Ошибка в процессе работы</t>
+  </si>
+  <si>
+    <t>Запрос данных для полки 1</t>
+  </si>
+  <si>
+    <t>Запрос данных для полки 2</t>
+  </si>
+  <si>
+    <t>Запрос данных для полки 3</t>
+  </si>
+  <si>
+    <t>Запрос данных для полки 4</t>
+  </si>
+  <si>
+    <t>Состояние захвата 1</t>
+  </si>
+  <si>
+    <t>Состояние захвата 2</t>
+  </si>
+  <si>
+    <t>Состояние патрона 1</t>
+  </si>
+  <si>
+    <t>Состояние патрона 2</t>
+  </si>
+  <si>
+    <t>Обработано деталей</t>
+  </si>
+  <si>
+    <t>Данные подготовлены для загрузки</t>
+  </si>
+  <si>
+    <t>Полка 1 включена</t>
+  </si>
+  <si>
+    <t>Полка 2 включена</t>
+  </si>
+  <si>
+    <t>Полка 3 включена</t>
+  </si>
+  <si>
+    <t>Полка 4 включена</t>
+  </si>
+  <si>
+    <t>Работа с полкой 1 завершена</t>
+  </si>
+  <si>
+    <t>Работа с полкой 2 завершена</t>
+  </si>
+  <si>
+    <t>Работа с полкой 3 завершена</t>
+  </si>
+  <si>
+    <t>Работа с полкой 4 завершена</t>
+  </si>
+  <si>
+    <t>Данные считаны</t>
   </si>
 </sst>
 </file>
@@ -1217,14 +1265,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1291,13 +1339,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="medium">
           <color theme="1"/>
         </top>
@@ -1321,6 +1362,13 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1892,7 +1940,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D433E639-47C8-435B-BE62-40BBD3A85586}" name="Таблица7" displayName="Таблица7" ref="A1:C66" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D433E639-47C8-435B-BE62-40BBD3A85586}" name="Таблица7" displayName="Таблица7" ref="A1:C66" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3">
   <autoFilter ref="A1:C66" xr:uid="{D433E639-47C8-435B-BE62-40BBD3A85586}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C0C4E1FE-6EA6-4426-AC8B-A634B9C978EE}" name="Адрес слова" dataDxfId="2"/>
@@ -2226,7 +2274,7 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="2" bestFit="1" customWidth="1"/>
@@ -2241,18 +2289,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2698,18 +2746,18 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="F20" s="4" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="F20" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -3174,11 +3222,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40895EFA-86F2-45C7-8EA9-6C33984E31A6}">
   <dimension ref="A1:I450"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="H2:I2"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -3188,24 +3236,24 @@
     <col min="6" max="6" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3778,7 +3826,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F22" s="1">
         <v>1084</v>
@@ -3808,7 +3856,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F23" s="1">
         <v>1085</v>
@@ -4584,10 +4632,6 @@
         <f t="shared" si="2"/>
         <v>P11031</v>
       </c>
-      <c r="H52" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> </v>
-      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
@@ -4601,6 +4645,9 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="D53" s="1" t="s">
+        <v>352</v>
+      </c>
       <c r="F53" s="1">
         <v>1115</v>
       </c>
@@ -4625,6 +4672,9 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="D54" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="F54" s="1">
         <v>1116</v>
       </c>
@@ -4636,6 +4686,9 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="I54" s="1" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
@@ -4649,6 +4702,9 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="D55" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="F55" s="1">
         <v>1117</v>
       </c>
@@ -4673,6 +4729,9 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="D56" s="1" t="s">
+        <v>355</v>
+      </c>
       <c r="F56" s="1">
         <v>1118</v>
       </c>
@@ -4697,6 +4756,9 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="D57" s="1" t="s">
+        <v>356</v>
+      </c>
       <c r="F57" s="1">
         <v>1119</v>
       </c>
@@ -4721,6 +4783,9 @@
         <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="D58" s="1" t="s">
+        <v>371</v>
+      </c>
       <c r="F58" s="1">
         <v>1120</v>
       </c>
@@ -4938,7 +5003,7 @@
         <v>P1004</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F67" s="1">
         <v>1129</v>
@@ -4952,7 +5017,7 @@
         <v>P1104</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>276</v>
+        <v>363</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -4968,7 +5033,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F68" s="1">
         <v>1130</v>
@@ -4982,7 +5047,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>277</v>
+        <v>364</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -4998,7 +5063,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F69" s="1">
         <v>1131</v>
@@ -5012,7 +5077,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>278</v>
+        <v>365</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -5028,7 +5093,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="F70" s="1">
         <v>1132</v>
@@ -5042,7 +5107,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>279</v>
+        <v>366</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -5058,7 +5123,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F71" s="1">
         <v>1133</v>
@@ -5072,7 +5137,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -5088,7 +5153,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F72" s="1">
         <v>1134</v>
@@ -5102,7 +5167,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -5118,7 +5183,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F73" s="1">
         <v>1135</v>
@@ -5132,7 +5197,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -5148,7 +5213,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F74" s="1">
         <v>1136</v>
@@ -5162,7 +5227,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -5189,7 +5254,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -5204,6 +5269,9 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="D76" s="1" t="s">
+        <v>367</v>
+      </c>
       <c r="F76" s="1">
         <v>1138</v>
       </c>
@@ -5228,6 +5296,9 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="D77" s="1" t="s">
+        <v>368</v>
+      </c>
       <c r="F77" s="1">
         <v>1139</v>
       </c>
@@ -5252,6 +5323,9 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="D78" s="1" t="s">
+        <v>369</v>
+      </c>
       <c r="F78" s="1">
         <v>1140</v>
       </c>
@@ -5276,6 +5350,9 @@
         <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
+      <c r="D79" s="1" t="s">
+        <v>370</v>
+      </c>
       <c r="F79" s="1">
         <v>1141</v>
       </c>
@@ -7292,6 +7369,9 @@
         <f t="shared" si="9"/>
         <v>P1010</v>
       </c>
+      <c r="D163" s="1" t="s">
+        <v>357</v>
+      </c>
       <c r="F163" s="1">
         <v>1225</v>
       </c>
@@ -7679,6 +7759,9 @@
         <f t="shared" si="9"/>
         <v>P1011</v>
       </c>
+      <c r="D179" s="1" t="s">
+        <v>358</v>
+      </c>
       <c r="F179" s="1">
         <v>1241</v>
       </c>
@@ -8063,6 +8146,9 @@
         <f t="shared" si="9"/>
         <v>P1012</v>
       </c>
+      <c r="D195" s="1" t="s">
+        <v>359</v>
+      </c>
       <c r="F195" s="1">
         <v>1257</v>
       </c>
@@ -8447,6 +8533,9 @@
         <f t="shared" si="14"/>
         <v>P1013</v>
       </c>
+      <c r="D211" s="1" t="s">
+        <v>360</v>
+      </c>
       <c r="F211" s="1">
         <v>1273</v>
       </c>
@@ -8830,6 +8919,9 @@
       <c r="C227" s="1" t="str">
         <f t="shared" si="14"/>
         <v>P1014</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>361</v>
       </c>
       <c r="F227" s="1">
         <v>1289</v>
@@ -14214,307 +14306,307 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA144AF3-4E40-4942-9302-D3CD0ABECF4D}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="C2" s="6" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="C20" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="C21" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="B22" s="4" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="C22" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>342</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="B23" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>348</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>349</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>322</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>